<commit_message>
Após intervenção do Copilot
</commit_message>
<xml_diff>
--- a/tests/mock_qpcr_results.xlsx
+++ b/tests/mock_qpcr_results.xlsx
@@ -582,7 +582,7 @@
         <v>52</v>
       </c>
       <c r="D2">
-        <v>15.44576122700076</v>
+        <v>29.91908308576159</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -596,7 +596,7 @@
         <v>53</v>
       </c>
       <c r="D3">
-        <v>23.3035576233585</v>
+        <v>15.78624825040675</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -610,7 +610,7 @@
         <v>54</v>
       </c>
       <c r="D4">
-        <v>15.62701041024309</v>
+        <v>25.99203707365621</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -638,7 +638,7 @@
         <v>56</v>
       </c>
       <c r="D6">
-        <v>23.86455482016488</v>
+        <v>28.36251929519641</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -652,7 +652,7 @@
         <v>57</v>
       </c>
       <c r="D7">
-        <v>26.59693582987767</v>
+        <v>27.33516258834177</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -666,7 +666,7 @@
         <v>58</v>
       </c>
       <c r="D8">
-        <v>29.43276958173749</v>
+        <v>27.90697549273979</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -694,7 +694,7 @@
         <v>59</v>
       </c>
       <c r="D10">
-        <v>29.03269602172377</v>
+        <v>17.83486287687179</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -708,7 +708,7 @@
         <v>52</v>
       </c>
       <c r="D11">
-        <v>19.12231214036628</v>
+        <v>15.32354943967238</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -722,7 +722,7 @@
         <v>53</v>
       </c>
       <c r="D12">
-        <v>21.96053354289874</v>
+        <v>24.08162849884349</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -736,7 +736,7 @@
         <v>54</v>
       </c>
       <c r="D13">
-        <v>21.00711072983367</v>
+        <v>28.6470164049419</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -764,7 +764,7 @@
         <v>56</v>
       </c>
       <c r="D15">
-        <v>19.66149413760995</v>
+        <v>23.36449009025481</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -778,7 +778,7 @@
         <v>57</v>
       </c>
       <c r="D16">
-        <v>24.44906125616487</v>
+        <v>15.45610409639018</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -792,7 +792,7 @@
         <v>58</v>
       </c>
       <c r="D17">
-        <v>27.42186607185155</v>
+        <v>20.05935655275456</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -820,7 +820,7 @@
         <v>59</v>
       </c>
       <c r="D19">
-        <v>22.56307312609785</v>
+        <v>16.24631882701703</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -834,7 +834,7 @@
         <v>52</v>
       </c>
       <c r="D20">
-        <v>26.08908442526056</v>
+        <v>18.17364171940874</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -848,7 +848,7 @@
         <v>53</v>
       </c>
       <c r="D21">
-        <v>25.68420537474084</v>
+        <v>23.03601881465361</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -862,7 +862,7 @@
         <v>54</v>
       </c>
       <c r="D22">
-        <v>25.23535586966773</v>
+        <v>20.35002070241994</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -890,7 +890,7 @@
         <v>56</v>
       </c>
       <c r="D24">
-        <v>21.16241078468732</v>
+        <v>28.25528284972551</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -904,7 +904,7 @@
         <v>57</v>
       </c>
       <c r="D25">
-        <v>21.89386855305323</v>
+        <v>29.05076991373071</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -918,7 +918,7 @@
         <v>58</v>
       </c>
       <c r="D26">
-        <v>17.98156479824935</v>
+        <v>22.6985507252763</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -946,7 +946,7 @@
         <v>59</v>
       </c>
       <c r="D28">
-        <v>24.7291100832586</v>
+        <v>21.9432244552801</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -960,7 +960,7 @@
         <v>52</v>
       </c>
       <c r="D29">
-        <v>19.14417730810192</v>
+        <v>24.10290603936804</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -974,7 +974,7 @@
         <v>53</v>
       </c>
       <c r="D30">
-        <v>20.76598092301661</v>
+        <v>25.22834291893694</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -988,7 +988,7 @@
         <v>54</v>
       </c>
       <c r="D31">
-        <v>25.9988918694599</v>
+        <v>26.54349713365851</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1016,7 +1016,7 @@
         <v>56</v>
       </c>
       <c r="D33">
-        <v>23.84922149721881</v>
+        <v>24.50448361294002</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1030,7 +1030,7 @@
         <v>57</v>
       </c>
       <c r="D34">
-        <v>19.24988837265671</v>
+        <v>16.99265825835865</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1044,7 +1044,7 @@
         <v>58</v>
       </c>
       <c r="D35">
-        <v>22.31371541037074</v>
+        <v>17.48521167235796</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1072,7 +1072,7 @@
         <v>59</v>
       </c>
       <c r="D37">
-        <v>28.59479033107965</v>
+        <v>26.17137333410349</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1086,7 +1086,7 @@
         <v>52</v>
       </c>
       <c r="D38">
-        <v>15.21969627942465</v>
+        <v>23.36892481713367</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1100,7 +1100,7 @@
         <v>53</v>
       </c>
       <c r="D39">
-        <v>17.61312196233431</v>
+        <v>21.64475020683657</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1114,7 +1114,7 @@
         <v>54</v>
       </c>
       <c r="D40">
-        <v>25.65646889120581</v>
+        <v>24.92069036888607</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1142,7 +1142,7 @@
         <v>56</v>
       </c>
       <c r="D42">
-        <v>17.29665045084383</v>
+        <v>17.01982911048585</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1156,7 +1156,7 @@
         <v>57</v>
       </c>
       <c r="D43">
-        <v>20.9953121906961</v>
+        <v>24.13116264648433</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1170,7 +1170,7 @@
         <v>58</v>
       </c>
       <c r="D44">
-        <v>27.3212352318164</v>
+        <v>15.61861857113046</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1198,7 +1198,7 @@
         <v>59</v>
       </c>
       <c r="D46">
-        <v>27.22715072456866</v>
+        <v>21.04715334847119</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1212,7 +1212,7 @@
         <v>52</v>
       </c>
       <c r="D47">
-        <v>16.865501162815</v>
+        <v>24.17973981870858</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1226,7 +1226,7 @@
         <v>53</v>
       </c>
       <c r="D48">
-        <v>23.41079837400995</v>
+        <v>25.06637829835389</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1240,7 +1240,7 @@
         <v>54</v>
       </c>
       <c r="D49">
-        <v>15.77794744310609</v>
+        <v>18.84516740422329</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1268,7 +1268,7 @@
         <v>56</v>
       </c>
       <c r="D51">
-        <v>18.1341483676238</v>
+        <v>19.71960692834739</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1282,7 +1282,7 @@
         <v>57</v>
       </c>
       <c r="D52">
-        <v>25.20597234095361</v>
+        <v>26.85156496323882</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1296,7 +1296,7 @@
         <v>58</v>
       </c>
       <c r="D53">
-        <v>22.85194956996985</v>
+        <v>29.4072463907693</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1324,7 +1324,7 @@
         <v>59</v>
       </c>
       <c r="D55">
-        <v>17.59732387422132</v>
+        <v>19.06214689585455</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1338,7 +1338,7 @@
         <v>52</v>
       </c>
       <c r="D56">
-        <v>21.2832732895958</v>
+        <v>16.33978423108259</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1352,7 +1352,7 @@
         <v>53</v>
       </c>
       <c r="D57">
-        <v>28.11653181514252</v>
+        <v>24.53072099267285</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1366,7 +1366,7 @@
         <v>54</v>
       </c>
       <c r="D58">
-        <v>18.42583880494109</v>
+        <v>20.65387719623434</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1394,7 +1394,7 @@
         <v>56</v>
       </c>
       <c r="D60">
-        <v>19.0756152655036</v>
+        <v>29.51997583114958</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -1408,7 +1408,7 @@
         <v>57</v>
       </c>
       <c r="D61">
-        <v>25.12406013596719</v>
+        <v>17.38585440071839</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1422,7 +1422,7 @@
         <v>58</v>
       </c>
       <c r="D62">
-        <v>17.4817800440983</v>
+        <v>22.55386212937888</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -1450,7 +1450,7 @@
         <v>59</v>
       </c>
       <c r="D64">
-        <v>15.66712950187304</v>
+        <v>20.41830362315221</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -1464,7 +1464,7 @@
         <v>52</v>
       </c>
       <c r="D65">
-        <v>19.59012745803476</v>
+        <v>21.60293479152927</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1478,7 +1478,7 @@
         <v>53</v>
       </c>
       <c r="D66">
-        <v>15.81589524124975</v>
+        <v>29.42166102232875</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -1492,7 +1492,7 @@
         <v>54</v>
       </c>
       <c r="D67">
-        <v>17.53788111795446</v>
+        <v>18.37185251796356</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -1520,7 +1520,7 @@
         <v>56</v>
       </c>
       <c r="D69">
-        <v>29.92888296109679</v>
+        <v>15.15543187556853</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -1534,7 +1534,7 @@
         <v>57</v>
       </c>
       <c r="D70">
-        <v>21.85488745335672</v>
+        <v>15.35179805215398</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -1548,7 +1548,7 @@
         <v>58</v>
       </c>
       <c r="D71">
-        <v>27.39456894811672</v>
+        <v>17.92105696594532</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -1576,7 +1576,7 @@
         <v>59</v>
       </c>
       <c r="D73">
-        <v>27.18030841401472</v>
+        <v>23.67732809941992</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -1590,7 +1590,7 @@
         <v>52</v>
       </c>
       <c r="D74">
-        <v>18.04730091342603</v>
+        <v>18.34210001241087</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -1604,7 +1604,7 @@
         <v>53</v>
       </c>
       <c r="D75">
-        <v>21.47977902001131</v>
+        <v>22.28773989974808</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -1618,7 +1618,7 @@
         <v>54</v>
       </c>
       <c r="D76">
-        <v>17.64937269443231</v>
+        <v>29.35886338236472</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -1646,7 +1646,7 @@
         <v>56</v>
       </c>
       <c r="D78">
-        <v>20.0284795546336</v>
+        <v>28.07867600926541</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -1660,7 +1660,7 @@
         <v>57</v>
       </c>
       <c r="D79">
-        <v>17.0061815896029</v>
+        <v>26.95395199476881</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -1674,7 +1674,7 @@
         <v>58</v>
       </c>
       <c r="D80">
-        <v>20.73580151849592</v>
+        <v>15.55878591892097</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -1702,7 +1702,7 @@
         <v>59</v>
       </c>
       <c r="D82">
-        <v>22.06268218905406</v>
+        <v>23.41711049661649</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -1716,7 +1716,7 @@
         <v>52</v>
       </c>
       <c r="D83">
-        <v>24.86594692543273</v>
+        <v>22.30836140051404</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -1730,7 +1730,7 @@
         <v>53</v>
       </c>
       <c r="D84">
-        <v>23.02710136842793</v>
+        <v>18.91594547008269</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -1744,7 +1744,7 @@
         <v>54</v>
       </c>
       <c r="D85">
-        <v>24.00070458580224</v>
+        <v>17.69659010257844</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -1772,7 +1772,7 @@
         <v>56</v>
       </c>
       <c r="D87">
-        <v>23.19080607631382</v>
+        <v>18.81397611696601</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -1786,7 +1786,7 @@
         <v>57</v>
       </c>
       <c r="D88">
-        <v>25.92095741425064</v>
+        <v>20.13937082261472</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -1800,7 +1800,7 @@
         <v>58</v>
       </c>
       <c r="D89">
-        <v>18.94180464097092</v>
+        <v>23.71574592613597</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -1828,7 +1828,7 @@
         <v>59</v>
       </c>
       <c r="D91">
-        <v>15.94436806633241</v>
+        <v>17.51217602709664</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -1842,7 +1842,7 @@
         <v>52</v>
       </c>
       <c r="D92">
-        <v>18.69214954111414</v>
+        <v>20.85156833150109</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -1856,7 +1856,7 @@
         <v>53</v>
       </c>
       <c r="D93">
-        <v>22.93263009468108</v>
+        <v>29.43729615648518</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -1870,7 +1870,7 @@
         <v>54</v>
       </c>
       <c r="D94">
-        <v>25.94028703574834</v>
+        <v>15.0462278183454</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -1898,7 +1898,7 @@
         <v>56</v>
       </c>
       <c r="D96">
-        <v>15.53357769538702</v>
+        <v>26.8489005368511</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -1912,7 +1912,7 @@
         <v>57</v>
       </c>
       <c r="D97">
-        <v>17.40693838101723</v>
+        <v>17.25343671387277</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -1926,7 +1926,7 @@
         <v>58</v>
       </c>
       <c r="D98">
-        <v>23.19034894855758</v>
+        <v>28.97801531210598</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -1954,7 +1954,7 @@
         <v>59</v>
       </c>
       <c r="D100">
-        <v>24.88493858299497</v>
+        <v>20.28566703987979</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -1968,7 +1968,7 @@
         <v>52</v>
       </c>
       <c r="D101">
-        <v>23.58751590612567</v>
+        <v>29.75986878242593</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -1982,7 +1982,7 @@
         <v>53</v>
       </c>
       <c r="D102">
-        <v>27.98496060926528</v>
+        <v>28.96332176721162</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -1996,7 +1996,7 @@
         <v>54</v>
       </c>
       <c r="D103">
-        <v>26.50055861195325</v>
+        <v>29.17280047033849</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -2024,7 +2024,7 @@
         <v>56</v>
       </c>
       <c r="D105">
-        <v>15.75888058134653</v>
+        <v>25.72834356051582</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -2038,7 +2038,7 @@
         <v>57</v>
       </c>
       <c r="D106">
-        <v>19.4120968112139</v>
+        <v>26.16061775645734</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -2052,7 +2052,7 @@
         <v>58</v>
       </c>
       <c r="D107">
-        <v>26.48072219388577</v>
+        <v>22.50766266566439</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -2080,7 +2080,7 @@
         <v>59</v>
       </c>
       <c r="D109">
-        <v>16.57390648880082</v>
+        <v>20.9043189618484</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -2094,7 +2094,7 @@
         <v>52</v>
       </c>
       <c r="D110">
-        <v>16.35426358538774</v>
+        <v>27.33388154946222</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -2108,7 +2108,7 @@
         <v>53</v>
       </c>
       <c r="D111">
-        <v>22.64037085924903</v>
+        <v>24.78035272665866</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -2122,7 +2122,7 @@
         <v>54</v>
       </c>
       <c r="D112">
-        <v>25.66864462390075</v>
+        <v>20.90885937008758</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -2150,7 +2150,7 @@
         <v>56</v>
       </c>
       <c r="D114">
-        <v>21.78725295407889</v>
+        <v>15.20735803150392</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -2164,7 +2164,7 @@
         <v>57</v>
       </c>
       <c r="D115">
-        <v>17.52491523415557</v>
+        <v>17.10192993346362</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -2178,7 +2178,7 @@
         <v>58</v>
       </c>
       <c r="D116">
-        <v>19.86452820542652</v>
+        <v>27.39030136114701</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -2206,7 +2206,7 @@
         <v>59</v>
       </c>
       <c r="D118">
-        <v>23.31907699811277</v>
+        <v>29.69759676980304</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -2220,7 +2220,7 @@
         <v>52</v>
       </c>
       <c r="D119">
-        <v>29.4378252627312</v>
+        <v>16.86668526683219</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -2234,7 +2234,7 @@
         <v>53</v>
       </c>
       <c r="D120">
-        <v>24.89109720448721</v>
+        <v>21.11186130764921</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -2248,7 +2248,7 @@
         <v>54</v>
       </c>
       <c r="D121">
-        <v>24.72587980633146</v>
+        <v>24.5236122742737</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -2276,7 +2276,7 @@
         <v>56</v>
       </c>
       <c r="D123">
-        <v>25.71801429426373</v>
+        <v>23.66534839515305</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -2290,7 +2290,7 @@
         <v>57</v>
       </c>
       <c r="D124">
-        <v>22.41702465616281</v>
+        <v>18.47000574516723</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -2304,7 +2304,7 @@
         <v>58</v>
       </c>
       <c r="D125">
-        <v>21.89715956290039</v>
+        <v>20.58128247505118</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -2332,7 +2332,7 @@
         <v>59</v>
       </c>
       <c r="D127">
-        <v>18.95451099167418</v>
+        <v>22.9393327900457</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -2346,7 +2346,7 @@
         <v>52</v>
       </c>
       <c r="D128">
-        <v>24.52149676101484</v>
+        <v>26.87680459374418</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -2360,7 +2360,7 @@
         <v>53</v>
       </c>
       <c r="D129">
-        <v>22.0653599928544</v>
+        <v>21.78618587762162</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -2374,7 +2374,7 @@
         <v>54</v>
       </c>
       <c r="D130">
-        <v>20.94057498244769</v>
+        <v>18.39196974559998</v>
       </c>
     </row>
     <row r="131" spans="1:4">
@@ -2402,7 +2402,7 @@
         <v>56</v>
       </c>
       <c r="D132">
-        <v>21.52703329896558</v>
+        <v>22.88171275069013</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -2416,7 +2416,7 @@
         <v>57</v>
       </c>
       <c r="D133">
-        <v>29.75218806930686</v>
+        <v>15.11632920791713</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -2430,7 +2430,7 @@
         <v>58</v>
       </c>
       <c r="D134">
-        <v>15.61277735118836</v>
+        <v>29.3085860261442</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -2458,7 +2458,7 @@
         <v>59</v>
       </c>
       <c r="D136">
-        <v>24.48515099923661</v>
+        <v>29.31445160927417</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -2472,7 +2472,7 @@
         <v>52</v>
       </c>
       <c r="D137">
-        <v>18.4648871980945</v>
+        <v>22.86421189781946</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -2486,7 +2486,7 @@
         <v>53</v>
       </c>
       <c r="D138">
-        <v>17.44664266774016</v>
+        <v>24.69631425831831</v>
       </c>
     </row>
     <row r="139" spans="1:4">
@@ -2500,7 +2500,7 @@
         <v>54</v>
       </c>
       <c r="D139">
-        <v>16.09300831431072</v>
+        <v>29.05093486799479</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -2528,7 +2528,7 @@
         <v>56</v>
       </c>
       <c r="D141">
-        <v>15.21669765772776</v>
+        <v>18.31354806282721</v>
       </c>
     </row>
     <row r="142" spans="1:4">
@@ -2542,7 +2542,7 @@
         <v>57</v>
       </c>
       <c r="D142">
-        <v>15.08812174160624</v>
+        <v>21.28262798815005</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -2556,7 +2556,7 @@
         <v>58</v>
       </c>
       <c r="D143">
-        <v>24.16520843219625</v>
+        <v>20.0592665914588</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -2584,7 +2584,7 @@
         <v>59</v>
       </c>
       <c r="D145">
-        <v>20.28046357018362</v>
+        <v>29.28426330500028</v>
       </c>
     </row>
     <row r="146" spans="1:4">
@@ -2598,7 +2598,7 @@
         <v>52</v>
       </c>
       <c r="D146">
-        <v>19.90635737122941</v>
+        <v>20.38015702271683</v>
       </c>
     </row>
     <row r="147" spans="1:4">
@@ -2612,7 +2612,7 @@
         <v>53</v>
       </c>
       <c r="D147">
-        <v>20.80007422742887</v>
+        <v>20.21677083821535</v>
       </c>
     </row>
     <row r="148" spans="1:4">
@@ -2626,7 +2626,7 @@
         <v>54</v>
       </c>
       <c r="D148">
-        <v>22.75276921665711</v>
+        <v>15.96826145110981</v>
       </c>
     </row>
     <row r="149" spans="1:4">
@@ -2654,7 +2654,7 @@
         <v>56</v>
       </c>
       <c r="D150">
-        <v>23.59132854442173</v>
+        <v>27.74456440566424</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -2668,7 +2668,7 @@
         <v>57</v>
       </c>
       <c r="D151">
-        <v>19.91049495860545</v>
+        <v>18.82187526600055</v>
       </c>
     </row>
     <row r="152" spans="1:4">
@@ -2682,7 +2682,7 @@
         <v>58</v>
       </c>
       <c r="D152">
-        <v>23.26289038874076</v>
+        <v>15.38503368126938</v>
       </c>
     </row>
     <row r="153" spans="1:4">
@@ -2710,7 +2710,7 @@
         <v>59</v>
       </c>
       <c r="D154">
-        <v>25.40089122774665</v>
+        <v>16.28115737978866</v>
       </c>
     </row>
     <row r="155" spans="1:4">
@@ -2724,7 +2724,7 @@
         <v>52</v>
       </c>
       <c r="D155">
-        <v>24.80447743656206</v>
+        <v>17.74283549788133</v>
       </c>
     </row>
     <row r="156" spans="1:4">
@@ -2738,7 +2738,7 @@
         <v>53</v>
       </c>
       <c r="D156">
-        <v>24.7403625986566</v>
+        <v>24.66214748948544</v>
       </c>
     </row>
     <row r="157" spans="1:4">
@@ -2752,7 +2752,7 @@
         <v>54</v>
       </c>
       <c r="D157">
-        <v>16.00185471540045</v>
+        <v>17.31366165666615</v>
       </c>
     </row>
     <row r="158" spans="1:4">
@@ -2780,7 +2780,7 @@
         <v>56</v>
       </c>
       <c r="D159">
-        <v>28.63925573703544</v>
+        <v>25.7169062532585</v>
       </c>
     </row>
     <row r="160" spans="1:4">
@@ -2794,7 +2794,7 @@
         <v>57</v>
       </c>
       <c r="D160">
-        <v>20.26530635281345</v>
+        <v>19.52502094187294</v>
       </c>
     </row>
     <row r="161" spans="1:4">
@@ -2808,7 +2808,7 @@
         <v>58</v>
       </c>
       <c r="D161">
-        <v>23.48579024173382</v>
+        <v>29.00841298134846</v>
       </c>
     </row>
     <row r="162" spans="1:4">
@@ -2836,7 +2836,7 @@
         <v>59</v>
       </c>
       <c r="D163">
-        <v>19.23041428017186</v>
+        <v>18.22590296636981</v>
       </c>
     </row>
     <row r="164" spans="1:4">
@@ -2850,7 +2850,7 @@
         <v>52</v>
       </c>
       <c r="D164">
-        <v>29.00261713505024</v>
+        <v>23.40150855435364</v>
       </c>
     </row>
     <row r="165" spans="1:4">
@@ -2864,7 +2864,7 @@
         <v>53</v>
       </c>
       <c r="D165">
-        <v>18.32286836997618</v>
+        <v>25.50046182574132</v>
       </c>
     </row>
     <row r="166" spans="1:4">
@@ -2878,7 +2878,7 @@
         <v>54</v>
       </c>
       <c r="D166">
-        <v>28.07227527793345</v>
+        <v>20.28094857488917</v>
       </c>
     </row>
     <row r="167" spans="1:4">
@@ -2906,7 +2906,7 @@
         <v>56</v>
       </c>
       <c r="D168">
-        <v>25.08715281556454</v>
+        <v>24.40838697500767</v>
       </c>
     </row>
     <row r="169" spans="1:4">
@@ -2920,7 +2920,7 @@
         <v>57</v>
       </c>
       <c r="D169">
-        <v>27.37599054472972</v>
+        <v>20.30882273147195</v>
       </c>
     </row>
     <row r="170" spans="1:4">
@@ -2934,7 +2934,7 @@
         <v>58</v>
       </c>
       <c r="D170">
-        <v>23.29095220765937</v>
+        <v>21.89813562395015</v>
       </c>
     </row>
     <row r="171" spans="1:4">
@@ -2962,7 +2962,7 @@
         <v>59</v>
       </c>
       <c r="D172">
-        <v>18.89869081207578</v>
+        <v>16.62477263622621</v>
       </c>
     </row>
     <row r="173" spans="1:4">
@@ -2976,7 +2976,7 @@
         <v>52</v>
       </c>
       <c r="D173">
-        <v>29.39710754689157</v>
+        <v>26.89903134322032</v>
       </c>
     </row>
     <row r="174" spans="1:4">
@@ -2990,7 +2990,7 @@
         <v>53</v>
       </c>
       <c r="D174">
-        <v>19.04660339573986</v>
+        <v>28.38438946945861</v>
       </c>
     </row>
     <row r="175" spans="1:4">
@@ -3004,7 +3004,7 @@
         <v>54</v>
       </c>
       <c r="D175">
-        <v>21.45901181837337</v>
+        <v>20.66549109927906</v>
       </c>
     </row>
     <row r="176" spans="1:4">
@@ -3032,7 +3032,7 @@
         <v>56</v>
       </c>
       <c r="D177">
-        <v>19.61377921395738</v>
+        <v>15.17319945464727</v>
       </c>
     </row>
     <row r="178" spans="1:4">
@@ -3046,7 +3046,7 @@
         <v>57</v>
       </c>
       <c r="D178">
-        <v>18.07121239454533</v>
+        <v>29.94288665541045</v>
       </c>
     </row>
     <row r="179" spans="1:4">
@@ -3060,7 +3060,7 @@
         <v>58</v>
       </c>
       <c r="D179">
-        <v>15.54058937089325</v>
+        <v>26.47573094641151</v>
       </c>
     </row>
     <row r="180" spans="1:4">
@@ -3088,7 +3088,7 @@
         <v>59</v>
       </c>
       <c r="D181">
-        <v>23.39603448019962</v>
+        <v>23.91022914727061</v>
       </c>
     </row>
     <row r="182" spans="1:4">
@@ -3102,7 +3102,7 @@
         <v>52</v>
       </c>
       <c r="D182">
-        <v>23.22578831484523</v>
+        <v>16.03353894847755</v>
       </c>
     </row>
     <row r="183" spans="1:4">
@@ -3116,7 +3116,7 @@
         <v>53</v>
       </c>
       <c r="D183">
-        <v>16.66154582876506</v>
+        <v>15.12671208135876</v>
       </c>
     </row>
     <row r="184" spans="1:4">
@@ -3130,7 +3130,7 @@
         <v>54</v>
       </c>
       <c r="D184">
-        <v>22.5858373867709</v>
+        <v>24.80715148771323</v>
       </c>
     </row>
     <row r="185" spans="1:4">
@@ -3158,7 +3158,7 @@
         <v>56</v>
       </c>
       <c r="D186">
-        <v>20.35687647438758</v>
+        <v>28.33946514244433</v>
       </c>
     </row>
     <row r="187" spans="1:4">
@@ -3172,7 +3172,7 @@
         <v>57</v>
       </c>
       <c r="D187">
-        <v>22.18487536752891</v>
+        <v>16.55544780599794</v>
       </c>
     </row>
     <row r="188" spans="1:4">
@@ -3186,7 +3186,7 @@
         <v>58</v>
       </c>
       <c r="D188">
-        <v>18.11692023649054</v>
+        <v>15.24022658661996</v>
       </c>
     </row>
     <row r="189" spans="1:4">
@@ -3214,7 +3214,7 @@
         <v>59</v>
       </c>
       <c r="D190">
-        <v>26.24273087857985</v>
+        <v>16.21359197838212</v>
       </c>
     </row>
     <row r="191" spans="1:4">
@@ -3228,7 +3228,7 @@
         <v>52</v>
       </c>
       <c r="D191">
-        <v>26.41433783238431</v>
+        <v>23.40006864379044</v>
       </c>
     </row>
     <row r="192" spans="1:4">
@@ -3242,7 +3242,7 @@
         <v>53</v>
       </c>
       <c r="D192">
-        <v>22.45213531987418</v>
+        <v>19.97517024427657</v>
       </c>
     </row>
     <row r="193" spans="1:4">
@@ -3256,7 +3256,7 @@
         <v>54</v>
       </c>
       <c r="D193">
-        <v>20.77891226549078</v>
+        <v>16.85656921315598</v>
       </c>
     </row>
     <row r="194" spans="1:4">
@@ -3284,7 +3284,7 @@
         <v>56</v>
       </c>
       <c r="D195">
-        <v>18.14275711422922</v>
+        <v>17.45955157642733</v>
       </c>
     </row>
     <row r="196" spans="1:4">
@@ -3298,7 +3298,7 @@
         <v>57</v>
       </c>
       <c r="D196">
-        <v>20.32600184968416</v>
+        <v>21.3578305933085</v>
       </c>
     </row>
     <row r="197" spans="1:4">
@@ -3312,7 +3312,7 @@
         <v>58</v>
       </c>
       <c r="D197">
-        <v>20.49437047747649</v>
+        <v>23.86702866046354</v>
       </c>
     </row>
     <row r="198" spans="1:4">
@@ -3340,7 +3340,7 @@
         <v>59</v>
       </c>
       <c r="D199">
-        <v>16.82096557703563</v>
+        <v>19.58301414869162</v>
       </c>
     </row>
     <row r="200" spans="1:4">
@@ -3354,7 +3354,7 @@
         <v>52</v>
       </c>
       <c r="D200">
-        <v>19.9314109691575</v>
+        <v>16.56427745247712</v>
       </c>
     </row>
     <row r="201" spans="1:4">
@@ -3368,7 +3368,7 @@
         <v>53</v>
       </c>
       <c r="D201">
-        <v>19.38930243330829</v>
+        <v>20.70122952880389</v>
       </c>
     </row>
     <row r="202" spans="1:4">
@@ -3382,7 +3382,7 @@
         <v>54</v>
       </c>
       <c r="D202">
-        <v>23.24679955919995</v>
+        <v>21.48126900880566</v>
       </c>
     </row>
     <row r="203" spans="1:4">
@@ -3410,7 +3410,7 @@
         <v>56</v>
       </c>
       <c r="D204">
-        <v>21.56190267872045</v>
+        <v>15.78149014012848</v>
       </c>
     </row>
     <row r="205" spans="1:4">
@@ -3424,7 +3424,7 @@
         <v>57</v>
       </c>
       <c r="D205">
-        <v>26.33429006381382</v>
+        <v>16.78521631861899</v>
       </c>
     </row>
     <row r="206" spans="1:4">
@@ -3438,7 +3438,7 @@
         <v>58</v>
       </c>
       <c r="D206">
-        <v>25.70655955116344</v>
+        <v>23.08270480443146</v>
       </c>
     </row>
     <row r="207" spans="1:4">
@@ -3466,7 +3466,7 @@
         <v>59</v>
       </c>
       <c r="D208">
-        <v>21.57276609393822</v>
+        <v>23.07189530694181</v>
       </c>
     </row>
     <row r="209" spans="1:4">
@@ -3480,7 +3480,7 @@
         <v>52</v>
       </c>
       <c r="D209">
-        <v>25.6596430765978</v>
+        <v>21.69022143507626</v>
       </c>
     </row>
     <row r="210" spans="1:4">
@@ -3494,7 +3494,7 @@
         <v>53</v>
       </c>
       <c r="D210">
-        <v>19.82142553688561</v>
+        <v>16.60875077737179</v>
       </c>
     </row>
     <row r="211" spans="1:4">
@@ -3508,7 +3508,7 @@
         <v>54</v>
       </c>
       <c r="D211">
-        <v>27.94003571322436</v>
+        <v>16.24236822080115</v>
       </c>
     </row>
     <row r="212" spans="1:4">
@@ -3536,7 +3536,7 @@
         <v>56</v>
       </c>
       <c r="D213">
-        <v>22.0352959321057</v>
+        <v>15.77641640870812</v>
       </c>
     </row>
     <row r="214" spans="1:4">
@@ -3550,7 +3550,7 @@
         <v>57</v>
       </c>
       <c r="D214">
-        <v>24.56358747782178</v>
+        <v>23.62568746575329</v>
       </c>
     </row>
     <row r="215" spans="1:4">
@@ -3564,7 +3564,7 @@
         <v>58</v>
       </c>
       <c r="D215">
-        <v>21.8578489459992</v>
+        <v>16.92411301145827</v>
       </c>
     </row>
     <row r="216" spans="1:4">
@@ -3592,7 +3592,7 @@
         <v>59</v>
       </c>
       <c r="D217">
-        <v>22.54611264569448</v>
+        <v>25.11264690681422</v>
       </c>
     </row>
     <row r="218" spans="1:4">
@@ -3606,7 +3606,7 @@
         <v>52</v>
       </c>
       <c r="D218">
-        <v>19.60015812338951</v>
+        <v>17.45860314825752</v>
       </c>
     </row>
     <row r="219" spans="1:4">
@@ -3620,7 +3620,7 @@
         <v>53</v>
       </c>
       <c r="D219">
-        <v>19.33805806696289</v>
+        <v>28.25156278895716</v>
       </c>
     </row>
     <row r="220" spans="1:4">
@@ -3634,7 +3634,7 @@
         <v>54</v>
       </c>
       <c r="D220">
-        <v>21.45841839141132</v>
+        <v>24.17976767497799</v>
       </c>
     </row>
     <row r="221" spans="1:4">
@@ -3662,7 +3662,7 @@
         <v>56</v>
       </c>
       <c r="D222">
-        <v>20.66987320810924</v>
+        <v>17.09296948693502</v>
       </c>
     </row>
     <row r="223" spans="1:4">
@@ -3676,7 +3676,7 @@
         <v>57</v>
       </c>
       <c r="D223">
-        <v>23.65647303602735</v>
+        <v>21.32752444252376</v>
       </c>
     </row>
     <row r="224" spans="1:4">
@@ -3690,7 +3690,7 @@
         <v>58</v>
       </c>
       <c r="D224">
-        <v>29.11496727552745</v>
+        <v>16.95038202471236</v>
       </c>
     </row>
     <row r="225" spans="1:4">
@@ -3718,7 +3718,7 @@
         <v>59</v>
       </c>
       <c r="D226">
-        <v>23.84462239492277</v>
+        <v>22.83672309485534</v>
       </c>
     </row>
     <row r="227" spans="1:4">
@@ -3732,7 +3732,7 @@
         <v>52</v>
       </c>
       <c r="D227">
-        <v>18.28743961973746</v>
+        <v>24.97392214707798</v>
       </c>
     </row>
     <row r="228" spans="1:4">
@@ -3746,7 +3746,7 @@
         <v>53</v>
       </c>
       <c r="D228">
-        <v>24.41714141904333</v>
+        <v>28.47121120221897</v>
       </c>
     </row>
     <row r="229" spans="1:4">
@@ -3760,7 +3760,7 @@
         <v>54</v>
       </c>
       <c r="D229">
-        <v>25.43522087137936</v>
+        <v>22.0753580519628</v>
       </c>
     </row>
     <row r="230" spans="1:4">
@@ -3788,7 +3788,7 @@
         <v>56</v>
       </c>
       <c r="D231">
-        <v>26.25283857062714</v>
+        <v>17.90194716266376</v>
       </c>
     </row>
     <row r="232" spans="1:4">
@@ -3802,7 +3802,7 @@
         <v>57</v>
       </c>
       <c r="D232">
-        <v>27.63052216010135</v>
+        <v>21.94407437079049</v>
       </c>
     </row>
     <row r="233" spans="1:4">
@@ -3816,7 +3816,7 @@
         <v>58</v>
       </c>
       <c r="D233">
-        <v>29.83583988344112</v>
+        <v>26.85570161041259</v>
       </c>
     </row>
     <row r="234" spans="1:4">
@@ -3844,7 +3844,7 @@
         <v>59</v>
       </c>
       <c r="D235">
-        <v>27.31992019426634</v>
+        <v>22.0239310913067</v>
       </c>
     </row>
     <row r="236" spans="1:4">
@@ -3858,7 +3858,7 @@
         <v>52</v>
       </c>
       <c r="D236">
-        <v>20.41898019766505</v>
+        <v>21.24570923545097</v>
       </c>
     </row>
     <row r="237" spans="1:4">
@@ -3872,7 +3872,7 @@
         <v>53</v>
       </c>
       <c r="D237">
-        <v>29.21456811338419</v>
+        <v>28.57307434900337</v>
       </c>
     </row>
     <row r="238" spans="1:4">
@@ -3886,7 +3886,7 @@
         <v>54</v>
       </c>
       <c r="D238">
-        <v>21.79041700495844</v>
+        <v>23.12077595934372</v>
       </c>
     </row>
     <row r="239" spans="1:4">
@@ -3914,7 +3914,7 @@
         <v>56</v>
       </c>
       <c r="D240">
-        <v>15.38950041414093</v>
+        <v>26.18726383187972</v>
       </c>
     </row>
     <row r="241" spans="1:4">
@@ -3928,7 +3928,7 @@
         <v>57</v>
       </c>
       <c r="D241">
-        <v>23.25663766162317</v>
+        <v>24.25583781844933</v>
       </c>
     </row>
     <row r="242" spans="1:4">
@@ -3942,7 +3942,7 @@
         <v>58</v>
       </c>
       <c r="D242">
-        <v>24.34939044448436</v>
+        <v>28.40104525474115</v>
       </c>
     </row>
     <row r="243" spans="1:4">
@@ -3970,7 +3970,7 @@
         <v>59</v>
       </c>
       <c r="D244">
-        <v>19.40707976262471</v>
+        <v>28.09768599228608</v>
       </c>
     </row>
     <row r="245" spans="1:4">
@@ -3984,7 +3984,7 @@
         <v>52</v>
       </c>
       <c r="D245">
-        <v>19.79135193828836</v>
+        <v>23.17192808839181</v>
       </c>
     </row>
     <row r="246" spans="1:4">
@@ -3998,7 +3998,7 @@
         <v>53</v>
       </c>
       <c r="D246">
-        <v>21.6539080462826</v>
+        <v>22.30440661348592</v>
       </c>
     </row>
     <row r="247" spans="1:4">
@@ -4012,7 +4012,7 @@
         <v>54</v>
       </c>
       <c r="D247">
-        <v>27.79817375125995</v>
+        <v>23.28695274629668</v>
       </c>
     </row>
     <row r="248" spans="1:4">
@@ -4040,7 +4040,7 @@
         <v>56</v>
       </c>
       <c r="D249">
-        <v>21.02640340724893</v>
+        <v>26.30192297625323</v>
       </c>
     </row>
     <row r="250" spans="1:4">
@@ -4054,7 +4054,7 @@
         <v>57</v>
       </c>
       <c r="D250">
-        <v>18.8353296953006</v>
+        <v>16.89675333614562</v>
       </c>
     </row>
     <row r="251" spans="1:4">
@@ -4068,7 +4068,7 @@
         <v>58</v>
       </c>
       <c r="D251">
-        <v>18.21380334418391</v>
+        <v>18.95376469126186</v>
       </c>
     </row>
     <row r="252" spans="1:4">
@@ -4096,7 +4096,7 @@
         <v>59</v>
       </c>
       <c r="D253">
-        <v>15.19484631293089</v>
+        <v>28.7432474381286</v>
       </c>
     </row>
     <row r="254" spans="1:4">
@@ -4110,7 +4110,7 @@
         <v>52</v>
       </c>
       <c r="D254">
-        <v>16.11909274864387</v>
+        <v>23.9739175088486</v>
       </c>
     </row>
     <row r="255" spans="1:4">
@@ -4124,7 +4124,7 @@
         <v>53</v>
       </c>
       <c r="D255">
-        <v>22.25003159703296</v>
+        <v>17.20866696304415</v>
       </c>
     </row>
     <row r="256" spans="1:4">
@@ -4138,7 +4138,7 @@
         <v>54</v>
       </c>
       <c r="D256">
-        <v>21.21669395152405</v>
+        <v>23.31573078508988</v>
       </c>
     </row>
     <row r="257" spans="1:4">
@@ -4166,7 +4166,7 @@
         <v>56</v>
       </c>
       <c r="D258">
-        <v>15.94824617238237</v>
+        <v>22.65475848852653</v>
       </c>
     </row>
     <row r="259" spans="1:4">
@@ -4180,7 +4180,7 @@
         <v>57</v>
       </c>
       <c r="D259">
-        <v>17.86264925229101</v>
+        <v>16.36029753212494</v>
       </c>
     </row>
     <row r="260" spans="1:4">
@@ -4194,7 +4194,7 @@
         <v>58</v>
       </c>
       <c r="D260">
-        <v>23.9137604950314</v>
+        <v>28.41328914191281</v>
       </c>
     </row>
     <row r="261" spans="1:4">
@@ -4222,7 +4222,7 @@
         <v>59</v>
       </c>
       <c r="D262">
-        <v>27.64778824220226</v>
+        <v>22.78134611228877</v>
       </c>
     </row>
     <row r="263" spans="1:4">
@@ -4236,7 +4236,7 @@
         <v>52</v>
       </c>
       <c r="D263">
-        <v>23.63007575224157</v>
+        <v>26.24971062157664</v>
       </c>
     </row>
     <row r="264" spans="1:4">
@@ -4250,7 +4250,7 @@
         <v>53</v>
       </c>
       <c r="D264">
-        <v>28.43564939752488</v>
+        <v>24.33800874140724</v>
       </c>
     </row>
     <row r="265" spans="1:4">
@@ -4264,7 +4264,7 @@
         <v>54</v>
       </c>
       <c r="D265">
-        <v>24.94931050625033</v>
+        <v>16.3273181489902</v>
       </c>
     </row>
     <row r="266" spans="1:4">
@@ -4292,7 +4292,7 @@
         <v>56</v>
       </c>
       <c r="D267">
-        <v>23.8853321738352</v>
+        <v>19.56765126292719</v>
       </c>
     </row>
     <row r="268" spans="1:4">
@@ -4306,7 +4306,7 @@
         <v>57</v>
       </c>
       <c r="D268">
-        <v>28.83634735636085</v>
+        <v>22.91196287038155</v>
       </c>
     </row>
     <row r="269" spans="1:4">
@@ -4320,7 +4320,7 @@
         <v>58</v>
       </c>
       <c r="D269">
-        <v>23.10708912938479</v>
+        <v>23.67686096871855</v>
       </c>
     </row>
     <row r="270" spans="1:4">
@@ -4348,7 +4348,7 @@
         <v>59</v>
       </c>
       <c r="D271">
-        <v>28.35009693621777</v>
+        <v>28.0968006360872</v>
       </c>
     </row>
     <row r="272" spans="1:4">
@@ -4362,7 +4362,7 @@
         <v>52</v>
       </c>
       <c r="D272">
-        <v>29.17635986745753</v>
+        <v>24.03869262600426</v>
       </c>
     </row>
     <row r="273" spans="1:4">
@@ -4376,7 +4376,7 @@
         <v>53</v>
       </c>
       <c r="D273">
-        <v>25.21466960695183</v>
+        <v>27.28230069227111</v>
       </c>
     </row>
     <row r="274" spans="1:4">
@@ -4390,7 +4390,7 @@
         <v>54</v>
       </c>
       <c r="D274">
-        <v>25.53627328691741</v>
+        <v>26.10981694476456</v>
       </c>
     </row>
     <row r="275" spans="1:4">
@@ -4418,7 +4418,7 @@
         <v>56</v>
       </c>
       <c r="D276">
-        <v>21.97992016108893</v>
+        <v>29.92349425263042</v>
       </c>
     </row>
     <row r="277" spans="1:4">
@@ -4432,7 +4432,7 @@
         <v>57</v>
       </c>
       <c r="D277">
-        <v>27.28327112059705</v>
+        <v>17.49183636206687</v>
       </c>
     </row>
     <row r="278" spans="1:4">
@@ -4446,7 +4446,7 @@
         <v>58</v>
       </c>
       <c r="D278">
-        <v>19.70642845038054</v>
+        <v>15.78710592496891</v>
       </c>
     </row>
     <row r="279" spans="1:4">
@@ -4474,7 +4474,7 @@
         <v>59</v>
       </c>
       <c r="D280">
-        <v>22.84884222929561</v>
+        <v>28.84045756504241</v>
       </c>
     </row>
     <row r="281" spans="1:4">
@@ -4488,7 +4488,7 @@
         <v>52</v>
       </c>
       <c r="D281">
-        <v>18.8203213324621</v>
+        <v>23.27318511200339</v>
       </c>
     </row>
     <row r="282" spans="1:4">
@@ -4502,7 +4502,7 @@
         <v>53</v>
       </c>
       <c r="D282">
-        <v>19.6755632653148</v>
+        <v>29.16801676165956</v>
       </c>
     </row>
     <row r="283" spans="1:4">
@@ -4516,7 +4516,7 @@
         <v>54</v>
       </c>
       <c r="D283">
-        <v>28.82947866142472</v>
+        <v>21.861742640303</v>
       </c>
     </row>
     <row r="284" spans="1:4">
@@ -4544,7 +4544,7 @@
         <v>56</v>
       </c>
       <c r="D285">
-        <v>22.55845386221359</v>
+        <v>18.593704591872</v>
       </c>
     </row>
     <row r="286" spans="1:4">
@@ -4558,7 +4558,7 @@
         <v>57</v>
       </c>
       <c r="D286">
-        <v>18.38319892953731</v>
+        <v>19.37324147359199</v>
       </c>
     </row>
     <row r="287" spans="1:4">
@@ -4572,7 +4572,7 @@
         <v>58</v>
       </c>
       <c r="D287">
-        <v>22.85183548085275</v>
+        <v>28.15913537327857</v>
       </c>
     </row>
     <row r="288" spans="1:4">
@@ -4600,7 +4600,7 @@
         <v>59</v>
       </c>
       <c r="D289">
-        <v>27.81247504673989</v>
+        <v>22.07052402706232</v>
       </c>
     </row>
     <row r="290" spans="1:4">
@@ -4614,7 +4614,7 @@
         <v>52</v>
       </c>
       <c r="D290">
-        <v>28.18038981029888</v>
+        <v>21.67716860059103</v>
       </c>
     </row>
     <row r="291" spans="1:4">
@@ -4628,7 +4628,7 @@
         <v>53</v>
       </c>
       <c r="D291">
-        <v>16.25618422524841</v>
+        <v>22.95562144184265</v>
       </c>
     </row>
     <row r="292" spans="1:4">
@@ -4642,7 +4642,7 @@
         <v>54</v>
       </c>
       <c r="D292">
-        <v>23.1457168828364</v>
+        <v>25.64148987328586</v>
       </c>
     </row>
     <row r="293" spans="1:4">
@@ -4670,7 +4670,7 @@
         <v>56</v>
       </c>
       <c r="D294">
-        <v>15.54766752894793</v>
+        <v>16.50164804137305</v>
       </c>
     </row>
     <row r="295" spans="1:4">
@@ -4684,7 +4684,7 @@
         <v>57</v>
       </c>
       <c r="D295">
-        <v>16.50632138604662</v>
+        <v>16.82912842216927</v>
       </c>
     </row>
     <row r="296" spans="1:4">
@@ -4698,7 +4698,7 @@
         <v>58</v>
       </c>
       <c r="D296">
-        <v>17.8360366135424</v>
+        <v>28.53572343669801</v>
       </c>
     </row>
     <row r="297" spans="1:4">
@@ -4726,7 +4726,7 @@
         <v>59</v>
       </c>
       <c r="D298">
-        <v>19.07803130350709</v>
+        <v>15.65813086826016</v>
       </c>
     </row>
     <row r="299" spans="1:4">
@@ -4740,7 +4740,7 @@
         <v>52</v>
       </c>
       <c r="D299">
-        <v>20.79378009490696</v>
+        <v>29.29401180729159</v>
       </c>
     </row>
     <row r="300" spans="1:4">
@@ -4754,7 +4754,7 @@
         <v>53</v>
       </c>
       <c r="D300">
-        <v>25.15090592353757</v>
+        <v>27.2413610876126</v>
       </c>
     </row>
     <row r="301" spans="1:4">
@@ -4768,7 +4768,7 @@
         <v>54</v>
       </c>
       <c r="D301">
-        <v>27.85102208428313</v>
+        <v>28.9703284243901</v>
       </c>
     </row>
     <row r="302" spans="1:4">
@@ -4796,7 +4796,7 @@
         <v>56</v>
       </c>
       <c r="D303">
-        <v>19.17050149113739</v>
+        <v>26.84730224645636</v>
       </c>
     </row>
     <row r="304" spans="1:4">
@@ -4810,7 +4810,7 @@
         <v>57</v>
       </c>
       <c r="D304">
-        <v>19.81500830529859</v>
+        <v>25.62297496886157</v>
       </c>
     </row>
     <row r="305" spans="1:4">
@@ -4824,7 +4824,7 @@
         <v>58</v>
       </c>
       <c r="D305">
-        <v>17.81108488976414</v>
+        <v>16.4828997928432</v>
       </c>
     </row>
     <row r="306" spans="1:4">
@@ -4852,7 +4852,7 @@
         <v>59</v>
       </c>
       <c r="D307">
-        <v>29.24008226382239</v>
+        <v>17.57986397788567</v>
       </c>
     </row>
     <row r="308" spans="1:4">
@@ -4866,7 +4866,7 @@
         <v>52</v>
       </c>
       <c r="D308">
-        <v>22.07925348952704</v>
+        <v>19.70169275688609</v>
       </c>
     </row>
     <row r="309" spans="1:4">
@@ -4880,7 +4880,7 @@
         <v>53</v>
       </c>
       <c r="D309">
-        <v>27.9349879706748</v>
+        <v>21.10533771553025</v>
       </c>
     </row>
     <row r="310" spans="1:4">
@@ -4894,7 +4894,7 @@
         <v>54</v>
       </c>
       <c r="D310">
-        <v>18.41065518264174</v>
+        <v>24.65222338544629</v>
       </c>
     </row>
     <row r="311" spans="1:4">
@@ -4922,7 +4922,7 @@
         <v>56</v>
       </c>
       <c r="D312">
-        <v>19.78843180259071</v>
+        <v>26.23397837985165</v>
       </c>
     </row>
     <row r="313" spans="1:4">
@@ -4936,7 +4936,7 @@
         <v>57</v>
       </c>
       <c r="D313">
-        <v>25.1265572832658</v>
+        <v>25.21638372295846</v>
       </c>
     </row>
     <row r="314" spans="1:4">
@@ -4950,7 +4950,7 @@
         <v>58</v>
       </c>
       <c r="D314">
-        <v>22.96131424362876</v>
+        <v>17.92714091827379</v>
       </c>
     </row>
     <row r="315" spans="1:4">
@@ -4978,7 +4978,7 @@
         <v>59</v>
       </c>
       <c r="D316">
-        <v>25.17704404440124</v>
+        <v>21.1501046867253</v>
       </c>
     </row>
     <row r="317" spans="1:4">
@@ -4992,7 +4992,7 @@
         <v>52</v>
       </c>
       <c r="D317">
-        <v>22.66927873360012</v>
+        <v>24.50042389070022</v>
       </c>
     </row>
     <row r="318" spans="1:4">
@@ -5006,7 +5006,7 @@
         <v>53</v>
       </c>
       <c r="D318">
-        <v>23.93680223523653</v>
+        <v>18.28797332210383</v>
       </c>
     </row>
     <row r="319" spans="1:4">
@@ -5020,7 +5020,7 @@
         <v>54</v>
       </c>
       <c r="D319">
-        <v>25.3924313859175</v>
+        <v>23.57328669061656</v>
       </c>
     </row>
     <row r="320" spans="1:4">
@@ -5048,7 +5048,7 @@
         <v>56</v>
       </c>
       <c r="D321">
-        <v>22.92376179351203</v>
+        <v>25.67165848436656</v>
       </c>
     </row>
     <row r="322" spans="1:4">
@@ -5062,7 +5062,7 @@
         <v>57</v>
       </c>
       <c r="D322">
-        <v>19.96943976560336</v>
+        <v>17.57174499273654</v>
       </c>
     </row>
     <row r="323" spans="1:4">
@@ -5076,7 +5076,7 @@
         <v>58</v>
       </c>
       <c r="D323">
-        <v>21.94961443718262</v>
+        <v>15.38083448515238</v>
       </c>
     </row>
     <row r="324" spans="1:4">
@@ -5104,7 +5104,7 @@
         <v>59</v>
       </c>
       <c r="D325">
-        <v>27.65389466182865</v>
+        <v>19.10495257484601</v>
       </c>
     </row>
     <row r="326" spans="1:4">
@@ -5118,7 +5118,7 @@
         <v>52</v>
       </c>
       <c r="D326">
-        <v>20.95056738030302</v>
+        <v>18.66836738814169</v>
       </c>
     </row>
     <row r="327" spans="1:4">
@@ -5132,7 +5132,7 @@
         <v>53</v>
       </c>
       <c r="D327">
-        <v>26.96386041581967</v>
+        <v>27.98064538639372</v>
       </c>
     </row>
     <row r="328" spans="1:4">
@@ -5146,7 +5146,7 @@
         <v>54</v>
       </c>
       <c r="D328">
-        <v>29.88569622919857</v>
+        <v>23.4435851815403</v>
       </c>
     </row>
     <row r="329" spans="1:4">
@@ -5174,7 +5174,7 @@
         <v>56</v>
       </c>
       <c r="D330">
-        <v>29.50842227225398</v>
+        <v>20.18248609084915</v>
       </c>
     </row>
     <row r="331" spans="1:4">
@@ -5188,7 +5188,7 @@
         <v>57</v>
       </c>
       <c r="D331">
-        <v>25.96853849240098</v>
+        <v>18.91663693878625</v>
       </c>
     </row>
     <row r="332" spans="1:4">
@@ -5202,7 +5202,7 @@
         <v>58</v>
       </c>
       <c r="D332">
-        <v>15.83921810448132</v>
+        <v>20.10871241980972</v>
       </c>
     </row>
     <row r="333" spans="1:4">
@@ -5230,7 +5230,7 @@
         <v>59</v>
       </c>
       <c r="D334">
-        <v>16.63493901483224</v>
+        <v>20.97837438539052</v>
       </c>
     </row>
     <row r="335" spans="1:4">
@@ -5244,7 +5244,7 @@
         <v>52</v>
       </c>
       <c r="D335">
-        <v>16.25387887615189</v>
+        <v>27.91604836336591</v>
       </c>
     </row>
     <row r="336" spans="1:4">
@@ -5258,7 +5258,7 @@
         <v>53</v>
       </c>
       <c r="D336">
-        <v>27.97621491854483</v>
+        <v>28.3481809032263</v>
       </c>
     </row>
     <row r="337" spans="1:4">
@@ -5272,7 +5272,7 @@
         <v>54</v>
       </c>
       <c r="D337">
-        <v>16.16527743987028</v>
+        <v>21.30668763593473</v>
       </c>
     </row>
     <row r="338" spans="1:4">
@@ -5300,7 +5300,7 @@
         <v>56</v>
       </c>
       <c r="D339">
-        <v>15.53552609732282</v>
+        <v>17.23691631934083</v>
       </c>
     </row>
     <row r="340" spans="1:4">
@@ -5314,7 +5314,7 @@
         <v>57</v>
       </c>
       <c r="D340">
-        <v>25.68108238896198</v>
+        <v>26.59334670978274</v>
       </c>
     </row>
     <row r="341" spans="1:4">
@@ -5328,7 +5328,7 @@
         <v>58</v>
       </c>
       <c r="D341">
-        <v>27.03739086531054</v>
+        <v>15.0486350871203</v>
       </c>
     </row>
     <row r="342" spans="1:4">
@@ -5356,7 +5356,7 @@
         <v>59</v>
       </c>
       <c r="D343">
-        <v>19.78062428994928</v>
+        <v>21.29926369873397</v>
       </c>
     </row>
     <row r="344" spans="1:4">
@@ -5370,7 +5370,7 @@
         <v>52</v>
       </c>
       <c r="D344">
-        <v>26.27325073031941</v>
+        <v>21.50767539818853</v>
       </c>
     </row>
     <row r="345" spans="1:4">
@@ -5384,7 +5384,7 @@
         <v>53</v>
       </c>
       <c r="D345">
-        <v>23.94501430512654</v>
+        <v>28.38616645357454</v>
       </c>
     </row>
     <row r="346" spans="1:4">
@@ -5398,7 +5398,7 @@
         <v>54</v>
       </c>
       <c r="D346">
-        <v>15.32401311006459</v>
+        <v>25.6786712043218</v>
       </c>
     </row>
     <row r="347" spans="1:4">
@@ -5426,7 +5426,7 @@
         <v>56</v>
       </c>
       <c r="D348">
-        <v>24.88856665798786</v>
+        <v>21.12348551296336</v>
       </c>
     </row>
     <row r="349" spans="1:4">
@@ -5440,7 +5440,7 @@
         <v>57</v>
       </c>
       <c r="D349">
-        <v>28.03580084827615</v>
+        <v>17.11517704304743</v>
       </c>
     </row>
     <row r="350" spans="1:4">
@@ -5454,7 +5454,7 @@
         <v>58</v>
       </c>
       <c r="D350">
-        <v>28.56238192412253</v>
+        <v>29.6912798259687</v>
       </c>
     </row>
     <row r="351" spans="1:4">
@@ -5482,7 +5482,7 @@
         <v>59</v>
       </c>
       <c r="D352">
-        <v>25.80138340126555</v>
+        <v>21.08268013050082</v>
       </c>
     </row>
     <row r="353" spans="1:4">
@@ -5496,7 +5496,7 @@
         <v>52</v>
       </c>
       <c r="D353">
-        <v>25.86898600008378</v>
+        <v>20.96916669508334</v>
       </c>
     </row>
     <row r="354" spans="1:4">
@@ -5510,7 +5510,7 @@
         <v>53</v>
       </c>
       <c r="D354">
-        <v>28.89290378655587</v>
+        <v>15.78204249501112</v>
       </c>
     </row>
     <row r="355" spans="1:4">
@@ -5524,7 +5524,7 @@
         <v>54</v>
       </c>
       <c r="D355">
-        <v>22.04957533047765</v>
+        <v>22.59060671057211</v>
       </c>
     </row>
     <row r="356" spans="1:4">
@@ -5552,7 +5552,7 @@
         <v>56</v>
       </c>
       <c r="D357">
-        <v>22.51697880921363</v>
+        <v>24.16931610046256</v>
       </c>
     </row>
     <row r="358" spans="1:4">
@@ -5566,7 +5566,7 @@
         <v>57</v>
       </c>
       <c r="D358">
-        <v>18.99719350202251</v>
+        <v>25.68344360697475</v>
       </c>
     </row>
     <row r="359" spans="1:4">
@@ -5580,7 +5580,7 @@
         <v>58</v>
       </c>
       <c r="D359">
-        <v>27.34822459673681</v>
+        <v>23.98605831743603</v>
       </c>
     </row>
     <row r="360" spans="1:4">
@@ -5608,7 +5608,7 @@
         <v>59</v>
       </c>
       <c r="D361">
-        <v>26.41969070007802</v>
+        <v>26.62749969827788</v>
       </c>
     </row>
     <row r="362" spans="1:4">
@@ -5622,7 +5622,7 @@
         <v>52</v>
       </c>
       <c r="D362">
-        <v>22.28482144957997</v>
+        <v>19.21716905264642</v>
       </c>
     </row>
     <row r="363" spans="1:4">
@@ -5636,7 +5636,7 @@
         <v>53</v>
       </c>
       <c r="D363">
-        <v>21.86062780383669</v>
+        <v>27.85411649506455</v>
       </c>
     </row>
     <row r="364" spans="1:4">
@@ -5650,7 +5650,7 @@
         <v>54</v>
       </c>
       <c r="D364">
-        <v>21.83114894762473</v>
+        <v>27.69804793183487</v>
       </c>
     </row>
     <row r="365" spans="1:4">
@@ -5678,7 +5678,7 @@
         <v>56</v>
       </c>
       <c r="D366">
-        <v>29.84563704017356</v>
+        <v>27.64359731215488</v>
       </c>
     </row>
     <row r="367" spans="1:4">
@@ -5692,7 +5692,7 @@
         <v>57</v>
       </c>
       <c r="D367">
-        <v>19.97125781519565</v>
+        <v>20.64105012946547</v>
       </c>
     </row>
     <row r="368" spans="1:4">
@@ -5706,7 +5706,7 @@
         <v>58</v>
       </c>
       <c r="D368">
-        <v>23.01462764466999</v>
+        <v>15.31120792831804</v>
       </c>
     </row>
     <row r="369" spans="1:4">
@@ -5734,7 +5734,7 @@
         <v>59</v>
       </c>
       <c r="D370">
-        <v>19.78584748774856</v>
+        <v>28.46727419856616</v>
       </c>
     </row>
     <row r="371" spans="1:4">
@@ -5748,7 +5748,7 @@
         <v>52</v>
       </c>
       <c r="D371">
-        <v>26.24015463503631</v>
+        <v>19.32448908504202</v>
       </c>
     </row>
     <row r="372" spans="1:4">
@@ -5762,7 +5762,7 @@
         <v>53</v>
       </c>
       <c r="D372">
-        <v>19.17582317513872</v>
+        <v>27.82142140876608</v>
       </c>
     </row>
     <row r="373" spans="1:4">
@@ -5776,7 +5776,7 @@
         <v>54</v>
       </c>
       <c r="D373">
-        <v>18.11101746141858</v>
+        <v>25.23212193509642</v>
       </c>
     </row>
     <row r="374" spans="1:4">
@@ -5804,7 +5804,7 @@
         <v>56</v>
       </c>
       <c r="D375">
-        <v>27.42103618669832</v>
+        <v>17.06423461161353</v>
       </c>
     </row>
     <row r="376" spans="1:4">
@@ -5818,7 +5818,7 @@
         <v>57</v>
       </c>
       <c r="D376">
-        <v>28.52982484653768</v>
+        <v>29.58510883085064</v>
       </c>
     </row>
     <row r="377" spans="1:4">
@@ -5832,7 +5832,7 @@
         <v>58</v>
       </c>
       <c r="D377">
-        <v>27.80341527087657</v>
+        <v>24.65141777643188</v>
       </c>
     </row>
     <row r="378" spans="1:4">
@@ -5860,7 +5860,7 @@
         <v>59</v>
       </c>
       <c r="D379">
-        <v>28.91616583842418</v>
+        <v>17.93600226598274</v>
       </c>
     </row>
     <row r="380" spans="1:4">
@@ -5874,7 +5874,7 @@
         <v>52</v>
       </c>
       <c r="D380">
-        <v>19.29259967923032</v>
+        <v>21.5464305683659</v>
       </c>
     </row>
     <row r="381" spans="1:4">
@@ -5888,7 +5888,7 @@
         <v>53</v>
       </c>
       <c r="D381">
-        <v>16.40492100785808</v>
+        <v>27.2585616981435</v>
       </c>
     </row>
     <row r="382" spans="1:4">
@@ -5902,7 +5902,7 @@
         <v>54</v>
       </c>
       <c r="D382">
-        <v>26.49818094540141</v>
+        <v>19.32073714075712</v>
       </c>
     </row>
     <row r="383" spans="1:4">
@@ -5930,7 +5930,7 @@
         <v>56</v>
       </c>
       <c r="D384">
-        <v>20.9899491131628</v>
+        <v>17.79684442733603</v>
       </c>
     </row>
     <row r="385" spans="1:4">
@@ -5944,7 +5944,7 @@
         <v>57</v>
       </c>
       <c r="D385">
-        <v>24.0207680888715</v>
+        <v>24.15784311797993</v>
       </c>
     </row>
     <row r="386" spans="1:4">
@@ -5958,7 +5958,7 @@
         <v>58</v>
       </c>
       <c r="D386">
-        <v>28.56537412101665</v>
+        <v>19.43823114938186</v>
       </c>
     </row>
     <row r="387" spans="1:4">
@@ -5986,7 +5986,7 @@
         <v>59</v>
       </c>
       <c r="D388">
-        <v>20.00310307275456</v>
+        <v>19.96931259556323</v>
       </c>
     </row>
     <row r="389" spans="1:4">
@@ -6000,7 +6000,7 @@
         <v>52</v>
       </c>
       <c r="D389">
-        <v>24.83228772660539</v>
+        <v>16.24515700571871</v>
       </c>
     </row>
     <row r="390" spans="1:4">
@@ -6014,7 +6014,7 @@
         <v>53</v>
       </c>
       <c r="D390">
-        <v>26.67521381943651</v>
+        <v>25.56703756931106</v>
       </c>
     </row>
     <row r="391" spans="1:4">
@@ -6028,7 +6028,7 @@
         <v>54</v>
       </c>
       <c r="D391">
-        <v>17.3032711074803</v>
+        <v>17.56433851692859</v>
       </c>
     </row>
     <row r="392" spans="1:4">
@@ -6056,7 +6056,7 @@
         <v>56</v>
       </c>
       <c r="D393">
-        <v>23.02542556819203</v>
+        <v>18.97466205553101</v>
       </c>
     </row>
     <row r="394" spans="1:4">
@@ -6070,7 +6070,7 @@
         <v>57</v>
       </c>
       <c r="D394">
-        <v>29.73960506381724</v>
+        <v>19.86993004353901</v>
       </c>
     </row>
     <row r="395" spans="1:4">
@@ -6084,7 +6084,7 @@
         <v>58</v>
       </c>
       <c r="D395">
-        <v>25.81046461507056</v>
+        <v>16.01613949324451</v>
       </c>
     </row>
     <row r="396" spans="1:4">
@@ -6112,7 +6112,7 @@
         <v>59</v>
       </c>
       <c r="D397">
-        <v>26.30795931736699</v>
+        <v>17.97034035512919</v>
       </c>
     </row>
     <row r="398" spans="1:4">
@@ -6126,7 +6126,7 @@
         <v>52</v>
       </c>
       <c r="D398">
-        <v>26.22400010506982</v>
+        <v>17.2341161525612</v>
       </c>
     </row>
     <row r="399" spans="1:4">
@@ -6140,7 +6140,7 @@
         <v>53</v>
       </c>
       <c r="D399">
-        <v>26.43405301468197</v>
+        <v>22.61672685525655</v>
       </c>
     </row>
     <row r="400" spans="1:4">
@@ -6154,7 +6154,7 @@
         <v>54</v>
       </c>
       <c r="D400">
-        <v>27.16485526184726</v>
+        <v>19.41400791726224</v>
       </c>
     </row>
     <row r="401" spans="1:4">
@@ -6182,7 +6182,7 @@
         <v>56</v>
       </c>
       <c r="D402">
-        <v>15.07662531953904</v>
+        <v>27.4651895931194</v>
       </c>
     </row>
     <row r="403" spans="1:4">
@@ -6196,7 +6196,7 @@
         <v>57</v>
       </c>
       <c r="D403">
-        <v>25.49315274563746</v>
+        <v>18.32629090418337</v>
       </c>
     </row>
     <row r="404" spans="1:4">
@@ -6210,7 +6210,7 @@
         <v>58</v>
       </c>
       <c r="D404">
-        <v>20.98208111000956</v>
+        <v>22.65672441360243</v>
       </c>
     </row>
     <row r="405" spans="1:4">
@@ -6238,7 +6238,7 @@
         <v>59</v>
       </c>
       <c r="D406">
-        <v>26.981581230975</v>
+        <v>18.62739691685163</v>
       </c>
     </row>
     <row r="407" spans="1:4">
@@ -6252,7 +6252,7 @@
         <v>52</v>
       </c>
       <c r="D407">
-        <v>28.27810401626104</v>
+        <v>19.66130001395607</v>
       </c>
     </row>
     <row r="408" spans="1:4">
@@ -6266,7 +6266,7 @@
         <v>53</v>
       </c>
       <c r="D408">
-        <v>19.72089682863848</v>
+        <v>22.83066342591465</v>
       </c>
     </row>
     <row r="409" spans="1:4">
@@ -6280,7 +6280,7 @@
         <v>54</v>
       </c>
       <c r="D409">
-        <v>29.39019276579683</v>
+        <v>18.37234587494583</v>
       </c>
     </row>
     <row r="410" spans="1:4">
@@ -6308,7 +6308,7 @@
         <v>56</v>
       </c>
       <c r="D411">
-        <v>19.71423107932794</v>
+        <v>20.92472880902053</v>
       </c>
     </row>
     <row r="412" spans="1:4">
@@ -6322,7 +6322,7 @@
         <v>57</v>
       </c>
       <c r="D412">
-        <v>23.12342178116741</v>
+        <v>25.42250423311717</v>
       </c>
     </row>
     <row r="413" spans="1:4">
@@ -6336,7 +6336,7 @@
         <v>58</v>
       </c>
       <c r="D413">
-        <v>25.6630853909363</v>
+        <v>22.1095147582515</v>
       </c>
     </row>
     <row r="414" spans="1:4">
@@ -6364,7 +6364,7 @@
         <v>59</v>
       </c>
       <c r="D415">
-        <v>21.58640329767115</v>
+        <v>23.772930102485</v>
       </c>
     </row>
     <row r="416" spans="1:4">
@@ -6378,7 +6378,7 @@
         <v>52</v>
       </c>
       <c r="D416">
-        <v>20.30232308552674</v>
+        <v>25.94679772757736</v>
       </c>
     </row>
     <row r="417" spans="1:4">
@@ -6392,7 +6392,7 @@
         <v>53</v>
       </c>
       <c r="D417">
-        <v>26.48939095734179</v>
+        <v>23.76609228050425</v>
       </c>
     </row>
     <row r="418" spans="1:4">
@@ -6406,7 +6406,7 @@
         <v>54</v>
       </c>
       <c r="D418">
-        <v>16.36606465973561</v>
+        <v>27.31403289693308</v>
       </c>
     </row>
     <row r="419" spans="1:4">
@@ -6434,7 +6434,7 @@
         <v>56</v>
       </c>
       <c r="D420">
-        <v>18.72594766628202</v>
+        <v>26.1372080004016</v>
       </c>
     </row>
     <row r="421" spans="1:4">
@@ -6448,7 +6448,7 @@
         <v>57</v>
       </c>
       <c r="D421">
-        <v>23.49194675564259</v>
+        <v>16.23236633078741</v>
       </c>
     </row>
     <row r="422" spans="1:4">
@@ -6462,7 +6462,7 @@
         <v>58</v>
       </c>
       <c r="D422">
-        <v>25.42490818109781</v>
+        <v>19.1590937242883</v>
       </c>
     </row>
     <row r="423" spans="1:4">
@@ -6490,7 +6490,7 @@
         <v>59</v>
       </c>
       <c r="D424">
-        <v>22.71380207065114</v>
+        <v>26.7073029518079</v>
       </c>
     </row>
     <row r="425" spans="1:4">
@@ -6504,7 +6504,7 @@
         <v>52</v>
       </c>
       <c r="D425">
-        <v>19.70306687767621</v>
+        <v>29.94711514636342</v>
       </c>
     </row>
     <row r="426" spans="1:4">
@@ -6518,7 +6518,7 @@
         <v>53</v>
       </c>
       <c r="D426">
-        <v>22.04339430765955</v>
+        <v>29.39739561125536</v>
       </c>
     </row>
     <row r="427" spans="1:4">
@@ -6532,7 +6532,7 @@
         <v>54</v>
       </c>
       <c r="D427">
-        <v>21.41251361062587</v>
+        <v>28.74600012613651</v>
       </c>
     </row>
     <row r="428" spans="1:4">
@@ -6560,7 +6560,7 @@
         <v>56</v>
       </c>
       <c r="D429">
-        <v>16.11693961153626</v>
+        <v>15.19392443178075</v>
       </c>
     </row>
     <row r="430" spans="1:4">
@@ -6574,7 +6574,7 @@
         <v>57</v>
       </c>
       <c r="D430">
-        <v>21.83369892089804</v>
+        <v>23.93586580676149</v>
       </c>
     </row>
     <row r="431" spans="1:4">
@@ -6588,7 +6588,7 @@
         <v>58</v>
       </c>
       <c r="D431">
-        <v>25.14702772326952</v>
+        <v>28.8984002761423</v>
       </c>
     </row>
     <row r="432" spans="1:4">
@@ -6616,7 +6616,7 @@
         <v>59</v>
       </c>
       <c r="D433">
-        <v>28.92480921972653</v>
+        <v>17.4637128038744</v>
       </c>
     </row>
   </sheetData>

</xml_diff>